<commit_message>
aggiornamento grafici venditore e regione
</commit_message>
<xml_diff>
--- a/Week4/Day3/day3-soluzioni-esercizi.xlsx
+++ b/Week4/Day3/day3-soluzioni-esercizi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A2F31E-C90F-5D4C-9076-C04A0B656571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE959C9-7EEA-FE4C-988B-2511EF912A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7060" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,36 +15,44 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sol-ese-1-giorno3'!$B$5:$G$75</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'sol-ese-1-giorno3'!$E$6:$E$162</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'sol-ese-1-giorno3'!$E$6:$E$162</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'sol-ese-1-giorno3'!$E$6:$E$162</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'sol-ese-1-giorno3'!$D$6:$D$162</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'sol-ese-1-giorno3'!$C$6:$C$162</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'sol-ese-1-giorno3'!$D$6:$D$162</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'sol-ese-1-giorno3'!$C$6:$C$162</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'sol-ese-1-giorno3'!$D$6:$D$162</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Foglio4!$M$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Foglio4!$L$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Foglio4!$L$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Foglio4!$M$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Foglio4!$L$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Foglio4!$N$10:$N$21</definedName>
     <definedName name="_xlchart.v1.28" hidden="1">Foglio4!$L$10:$M$21</definedName>
     <definedName name="_xlchart.v1.29" hidden="1">Foglio4!$N$10:$N$21</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Foglio4!$L$10:$M$21</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Foglio4!$N$10:$N$21</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'sol-ese-1-giorno3'!$E$6:$E$162</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'sol-ese-1-giorno3'!$C$6:$C$162</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'sol-ese-1-giorno3'!$G$6:$G$162</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Foglio4!$Q$10:$Q$17</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Foglio4!$S$10:$S$17</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Foglio4!$Q$10:$R$17</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Foglio4!$S$10:$S$17</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Foglio4!$L$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Foglio4!$Q$10:$R$17</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Foglio4!$S$10:$S$17</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Foglio4!$M$10:$M$21</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Foglio4!$N$10:$N$21</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'sol-2-ese-2-giorno3'!$J$17:$J$29</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">'sol-2-ese-2-giorno3'!$K$17:$K$29</definedName>
     <definedName name="_xlcn.WorksheetConnection_PivorbaseB2G1591" hidden="1">'sol-ese-1-giorno3'!$B$5:$G$162</definedName>
@@ -108,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="74">
   <si>
     <t>Venditore</t>
   </si>
@@ -602,6 +610,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Fatturato per venditore</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> e per regione</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -633,7 +671,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16652777777777777"/>
+          <c:y val="0.17168999708369789"/>
+          <c:w val="0.79736111111111108"/>
+          <c:h val="0.52189778361038208"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -651,6 +699,179 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-3504-8B48-864A-18A14883B35C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Foglio4!$L$10:$M$21</c:f>
@@ -927,15 +1148,592 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Fatturato per regione e per venditore</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio4!$T$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fatturato</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-BCED-D845-93E5-88CC8F26A56E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Foglio4!$R$10:$S$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>bianchi</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>verdi</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>rossi</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>neri</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>bianchi</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>verdi</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>rossi</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>neri</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>bianchi</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>verdi</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>rossi</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>neri</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>lombardia</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v> veneto </c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>friuli</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio4!$T$10:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>_-"€"\ * #,##0.00_-;\-"€"\ * #,##0.00_-;_-"€"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>39950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32920</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9377</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40174</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31038</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70478</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44030</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BCED-D845-93E5-88CC8F26A56E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1717937727"/>
+        <c:axId val="1717706607"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1717937727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1717706607"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1717706607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1717937727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1008,10 +1806,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.24</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1086,10 +1884,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1144,10 +1942,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1200,10 +1998,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.22</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1511,6 +2309,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="416">
   <cs:axisTitle>
@@ -4058,6 +4896,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5309,6 +6650,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>74145</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>159007</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>131405</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>39201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Grafico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4DCBA50-F8BD-3A98-0680-74925D46F63A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9404,10 +10781,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1A2957-AA6F-AD4C-A19E-3EDB12C78799}">
-  <dimension ref="A1:P158"/>
+  <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="173" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="K10" zoomScale="173" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9415,9 +10792,11 @@
     <col min="1" max="1" width="11.1640625" style="41" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" customWidth="1"/>
+    <col min="20" max="20" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>14</v>
       </c>
@@ -9437,7 +10816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="41">
         <v>44008</v>
       </c>
@@ -9457,7 +10836,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="41">
         <v>44008</v>
       </c>
@@ -9477,7 +10856,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="41">
         <v>44008</v>
       </c>
@@ -9497,7 +10876,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="41">
         <v>44011</v>
       </c>
@@ -9532,7 +10911,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="41">
         <v>44011</v>
       </c>
@@ -9571,7 +10950,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="41">
         <v>44011</v>
       </c>
@@ -9591,7 +10970,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="41">
         <v>44011</v>
       </c>
@@ -9611,7 +10990,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="41">
         <v>44013</v>
       </c>
@@ -9639,8 +11018,17 @@
       <c r="N9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="41">
         <v>44014</v>
       </c>
@@ -9669,8 +11057,18 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Bianchi",$C$2:$C$158,"Lombardia")</f>
         <v>39950</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S10" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="43">
+        <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Bianchi",$C$2:$C$158,"Lombardia")</f>
+        <v>39950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="41">
         <v>44015</v>
       </c>
@@ -9696,8 +11094,15 @@
         <f>SUMIFS(F2:F158,B2:B158,"Bianchi",C2:C158,"Veneto")</f>
         <v>70478</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" s="43">
+        <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Lombardia")</f>
+        <v>37960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="41">
         <v>44018</v>
       </c>
@@ -9723,8 +11128,15 @@
         <f>SUMIFS(F3:F159,B3:B159,"Bianchi",C3:C159,"Veneto")</f>
         <v>70478</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>69</v>
+      </c>
+      <c r="T12" s="43">
+        <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Rossi",$C$2:$C$158,"Lombardia")</f>
+        <v>32920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="41">
         <v>44018</v>
       </c>
@@ -9753,8 +11165,15 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Lombardia")</f>
         <v>37960</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>70</v>
+      </c>
+      <c r="T13" s="43">
+        <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Neri",$C$2:$C$158,"Lombardia")</f>
+        <v>9377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="41">
         <v>44018</v>
       </c>
@@ -9780,8 +11199,18 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Veneto")</f>
         <v>40174</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="S14" t="s">
+        <v>67</v>
+      </c>
+      <c r="T14" s="43">
+        <v>70478</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="41">
         <v>44019</v>
       </c>
@@ -9807,8 +11236,16 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Friuli")</f>
         <v>44030</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" t="s">
+        <v>68</v>
+      </c>
+      <c r="T15" s="43">
+        <v>40174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="41">
         <v>44019</v>
       </c>
@@ -9837,8 +11274,16 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Rossi",$C$2:$C$158,"Lombardia")</f>
         <v>32920</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" t="s">
+        <v>69</v>
+      </c>
+      <c r="T16" s="43">
+        <v>40174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="41">
         <v>44020</v>
       </c>
@@ -9864,8 +11309,16 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Veneto")</f>
         <v>40174</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" t="s">
+        <v>70</v>
+      </c>
+      <c r="T17" s="43">
+        <v>31038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="41">
         <v>44021</v>
       </c>
@@ -9891,8 +11344,18 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Verdi",$C$2:$C$158,"Friuli")</f>
         <v>44030</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q18" s="43"/>
+      <c r="R18" t="s">
+        <v>73</v>
+      </c>
+      <c r="S18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T18" s="43">
+        <v>70478</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="41">
         <v>44022</v>
       </c>
@@ -9921,8 +11384,15 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Neri",$C$2:$C$158,"Lombardia")</f>
         <v>9377</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q19" s="43"/>
+      <c r="S19" t="s">
+        <v>68</v>
+      </c>
+      <c r="T19" s="43">
+        <v>44030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="41">
         <v>44025</v>
       </c>
@@ -9948,8 +11418,15 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Neri",$C$2:$C$158,"Veneto")</f>
         <v>31038</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q20" s="43"/>
+      <c r="S20" t="s">
+        <v>69</v>
+      </c>
+      <c r="T20" s="43">
+        <v>44030</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="41">
         <v>44025</v>
       </c>
@@ -9975,8 +11452,16 @@
         <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Neri",$C$2:$C$158,"Friuli")</f>
         <v>45120</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q21" s="43"/>
+      <c r="S21" t="s">
+        <v>70</v>
+      </c>
+      <c r="T21" s="43">
+        <f>SUMIFS($F$2:$F$158,$B$2:$B$158,"Neri",$C$2:$C$158,"Friuli")</f>
+        <v>45120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="41">
         <v>44026</v>
       </c>
@@ -9996,7 +11481,7 @@
         <v>6240</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="41">
         <v>44027</v>
       </c>
@@ -10016,7 +11501,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="41">
         <v>44027</v>
       </c>
@@ -10036,7 +11521,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="41">
         <v>44027</v>
       </c>
@@ -10056,7 +11541,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
         <v>44028</v>
       </c>
@@ -10076,7 +11561,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="41">
         <v>44028</v>
       </c>
@@ -10096,7 +11581,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="41">
         <v>44028</v>
       </c>
@@ -10116,7 +11601,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="41">
         <v>44029</v>
       </c>
@@ -10136,7 +11621,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="41">
         <v>44029</v>
       </c>
@@ -10156,7 +11641,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="41">
         <v>44029</v>
       </c>
@@ -10176,7 +11661,7 @@
         <v>10160</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="41">
         <v>44029</v>
       </c>

</xml_diff>